<commit_message>
Update scripts to remove rownames
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s379011\surfdrive\projects\2020covid-19\covid-19\workflow\r_script\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s379011\surfdrive\projects\2020covid-19\covid-19\workflow\excess_mortality\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Berekening oversterfte" sheetId="1" r:id="rId1"/>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,17 +1105,32 @@
         <v>-189</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>31</v>
+      </c>
+      <c r="G23">
+        <v>2620</v>
+      </c>
+      <c r="H23">
+        <v>2944</v>
+      </c>
+      <c r="I23">
+        <f>G23-H23</f>
+        <v>-324</v>
+      </c>
+    </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
         <v>7</v>
       </c>
       <c r="G28" s="3">
-        <f>SUM(G3:G22)</f>
-        <v>65263</v>
+        <f>SUM(G3:G23)</f>
+        <v>67883</v>
       </c>
       <c r="H28" s="3">
-        <f>SUM(H3:H22)</f>
-        <v>58780</v>
+        <f>SUM(H3:H23)</f>
+        <v>61724</v>
       </c>
       <c r="I28" s="3">
         <f>SUM(I3:I22)</f>

</xml_diff>

<commit_message>
Update files excess mortality and add parse for cases_ggd_agegroups
Former-commit-id: 21fd39a7339dec48e2397f8f5984739b5604c078
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,10 +590,11 @@
         <v>3216</v>
       </c>
       <c r="H3">
-        <v>3051</v>
+        <v>3052</v>
       </c>
       <c r="I3">
-        <v>165</v>
+        <f>G3-H3</f>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -614,10 +615,11 @@
         <v>3612</v>
       </c>
       <c r="H4">
-        <v>3092</v>
+        <v>3093</v>
       </c>
       <c r="I4">
-        <v>520</v>
+        <f t="shared" ref="I4:I25" si="0">G4-H4</f>
+        <v>519</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -638,10 +640,11 @@
         <v>4458</v>
       </c>
       <c r="H5">
-        <v>3113</v>
+        <v>3114</v>
       </c>
       <c r="I5">
-        <v>1345</v>
+        <f t="shared" si="0"/>
+        <v>1344</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -662,10 +665,11 @@
         <v>5084</v>
       </c>
       <c r="H6">
-        <v>3113</v>
+        <v>3114</v>
       </c>
       <c r="I6">
-        <v>1971</v>
+        <f t="shared" si="0"/>
+        <v>1970</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -683,13 +687,14 @@
         <v>15</v>
       </c>
       <c r="G7">
-        <v>4974</v>
+        <v>4977</v>
       </c>
       <c r="H7">
-        <v>2907</v>
+        <v>2908</v>
       </c>
       <c r="I7">
-        <v>2067</v>
+        <f t="shared" si="0"/>
+        <v>2069</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -707,12 +712,13 @@
         <v>16</v>
       </c>
       <c r="G8">
-        <v>4298</v>
+        <v>4299</v>
       </c>
       <c r="H8">
-        <v>3008</v>
+        <v>3009</v>
       </c>
       <c r="I8">
+        <f t="shared" si="0"/>
         <v>1290</v>
       </c>
     </row>
@@ -731,13 +737,14 @@
         <v>17</v>
       </c>
       <c r="G9">
-        <v>3903</v>
+        <v>3905</v>
       </c>
       <c r="H9">
-        <v>2924</v>
+        <v>2925</v>
       </c>
       <c r="I9">
-        <v>979</v>
+        <f t="shared" si="0"/>
+        <v>980</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -755,12 +762,13 @@
         <v>18</v>
       </c>
       <c r="G10">
-        <v>3377</v>
+        <v>3378</v>
       </c>
       <c r="H10">
-        <v>2977</v>
+        <v>2978</v>
       </c>
       <c r="I10">
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
@@ -779,12 +787,13 @@
         <v>19</v>
       </c>
       <c r="G11">
-        <v>2980</v>
+        <v>2981</v>
       </c>
       <c r="H11">
-        <v>2931</v>
+        <v>2932</v>
       </c>
       <c r="I11">
+        <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
@@ -800,7 +809,7 @@
         <v>3215</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:D22" si="0">(100-(B12-AVERAGE(B$4:B$11)))/100</f>
+        <f t="shared" ref="D12:D22" si="1">(100-(B12-AVERAGE(B$4:B$11)))/100</f>
         <v>0.98019642857142852</v>
       </c>
       <c r="E12" s="3"/>
@@ -811,10 +820,11 @@
         <v>2772</v>
       </c>
       <c r="H12">
-        <v>3048</v>
+        <v>3049</v>
       </c>
       <c r="I12">
-        <v>-276</v>
+        <f t="shared" si="0"/>
+        <v>-277</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -829,7 +839,7 @@
         <v>3609</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.99333928571428576</v>
       </c>
       <c r="E13" s="3"/>
@@ -837,12 +847,13 @@
         <v>21</v>
       </c>
       <c r="G13">
-        <v>2767</v>
+        <v>2768</v>
       </c>
       <c r="H13">
-        <v>2809</v>
+        <v>2810</v>
       </c>
       <c r="I13">
+        <f t="shared" si="0"/>
         <v>-42</v>
       </c>
     </row>
@@ -858,7 +869,7 @@
         <v>4450</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0057678571428572</v>
       </c>
       <c r="E14" s="3"/>
@@ -866,13 +877,14 @@
         <v>22</v>
       </c>
       <c r="G14">
-        <v>2722</v>
+        <v>2724</v>
       </c>
       <c r="H14">
-        <v>2821</v>
+        <v>2822</v>
       </c>
       <c r="I14">
-        <v>-99</v>
+        <f t="shared" si="0"/>
+        <v>-98</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -887,7 +899,7 @@
         <v>5080</v>
       </c>
       <c r="D15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.001482142857143</v>
       </c>
       <c r="E15" s="3"/>
@@ -895,12 +907,13 @@
         <v>23</v>
       </c>
       <c r="G15">
-        <v>2680</v>
+        <v>2681</v>
       </c>
       <c r="H15">
-        <v>2859</v>
+        <v>2860</v>
       </c>
       <c r="I15">
+        <f t="shared" si="0"/>
         <v>-179</v>
       </c>
     </row>
@@ -916,7 +929,7 @@
         <v>4972</v>
       </c>
       <c r="D16" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.93405357142857159</v>
       </c>
       <c r="E16" s="3"/>
@@ -924,13 +937,14 @@
         <v>24</v>
       </c>
       <c r="G16">
-        <v>2688</v>
+        <v>2691</v>
       </c>
       <c r="H16">
-        <v>2805</v>
+        <v>2806</v>
       </c>
       <c r="I16">
-        <v>-117</v>
+        <f t="shared" si="0"/>
+        <v>-115</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -945,7 +959,7 @@
         <v>4292</v>
       </c>
       <c r="D17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.96648214285714285</v>
       </c>
       <c r="E17" s="3"/>
@@ -953,13 +967,14 @@
         <v>25</v>
       </c>
       <c r="G17">
-        <v>2688</v>
+        <v>2690</v>
       </c>
       <c r="H17">
-        <v>2890</v>
+        <v>2891</v>
       </c>
       <c r="I17">
-        <v>-202</v>
+        <f t="shared" si="0"/>
+        <v>-201</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -974,7 +989,7 @@
         <v>3893</v>
       </c>
       <c r="D18" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.93933928571428549</v>
       </c>
       <c r="E18" s="3"/>
@@ -982,13 +997,14 @@
         <v>26</v>
       </c>
       <c r="G18">
-        <v>2657</v>
+        <v>2659</v>
       </c>
       <c r="H18">
-        <v>3062</v>
+        <v>3063</v>
       </c>
       <c r="I18">
-        <v>-405</v>
+        <f t="shared" si="0"/>
+        <v>-404</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1003,7 +1019,7 @@
         <v>3368</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.95648214285714261</v>
       </c>
       <c r="E19" s="3"/>
@@ -1011,13 +1027,14 @@
         <v>27</v>
       </c>
       <c r="G19">
-        <v>2631</v>
+        <v>2633</v>
       </c>
       <c r="H19">
-        <v>2834</v>
+        <v>2835</v>
       </c>
       <c r="I19">
-        <v>-203</v>
+        <f t="shared" si="0"/>
+        <v>-202</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1032,7 +1049,7 @@
         <v>2964</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.9417678571428576</v>
       </c>
       <c r="E20" s="3"/>
@@ -1040,13 +1057,14 @@
         <v>28</v>
       </c>
       <c r="G20">
-        <v>2602</v>
+        <v>2610</v>
       </c>
       <c r="H20">
         <v>2855</v>
       </c>
       <c r="I20">
-        <v>-253</v>
+        <f t="shared" si="0"/>
+        <v>-245</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1061,20 +1079,21 @@
         <v>2735</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.97933928571428563</v>
       </c>
       <c r="F21">
         <v>29</v>
       </c>
       <c r="G21">
-        <v>2509</v>
+        <v>2519</v>
       </c>
       <c r="H21">
-        <v>2847</v>
+        <v>2848</v>
       </c>
       <c r="I21">
-        <v>-338</v>
+        <f t="shared" si="0"/>
+        <v>-329</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1088,7 +1107,7 @@
         <v>2759</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.90233928571428546</v>
       </c>
       <c r="E22" s="3"/>
@@ -1096,13 +1115,14 @@
         <v>30</v>
       </c>
       <c r="G22">
-        <v>2645</v>
+        <v>2666</v>
       </c>
       <c r="H22">
-        <v>2834</v>
+        <v>2835</v>
       </c>
       <c r="I22">
-        <v>-189</v>
+        <f t="shared" si="0"/>
+        <v>-169</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1110,14 +1130,44 @@
         <v>31</v>
       </c>
       <c r="G23">
-        <v>2620</v>
+        <v>2640</v>
       </c>
       <c r="H23">
         <v>2944</v>
       </c>
       <c r="I23">
-        <f>G23-H23</f>
-        <v>-324</v>
+        <f t="shared" si="0"/>
+        <v>-304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>32</v>
+      </c>
+      <c r="G24">
+        <v>2623</v>
+      </c>
+      <c r="H24">
+        <v>3103</v>
+      </c>
+      <c r="I24">
+        <f>G24-H24</f>
+        <v>-480</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>33</v>
+      </c>
+      <c r="G25">
+        <v>3172</v>
+      </c>
+      <c r="H25">
+        <v>3114</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1125,16 +1175,16 @@
         <v>7</v>
       </c>
       <c r="G28" s="3">
-        <f>SUM(G3:G23)</f>
-        <v>67883</v>
+        <f>SUM(G3:G25)</f>
+        <v>73758</v>
       </c>
       <c r="H28" s="3">
-        <f>SUM(H3:H23)</f>
-        <v>61724</v>
+        <f>SUM(H3:H25)</f>
+        <v>67960</v>
       </c>
       <c r="I28" s="3">
-        <f>SUM(I3:I22)</f>
-        <v>6483</v>
+        <f>SUM(I3:I25)</f>
+        <v>5798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update weekly excess mortality analyses
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>3052</v>
       </c>
       <c r="I3">
-        <f>G3-H3</f>
+        <f t="shared" ref="I3:I26" si="0">G3-H3</f>
         <v>164</v>
       </c>
     </row>
@@ -618,7 +618,7 @@
         <v>3093</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I25" si="0">G4-H4</f>
+        <f t="shared" si="0"/>
         <v>519</v>
       </c>
     </row>
@@ -787,14 +787,14 @@
         <v>19</v>
       </c>
       <c r="G11">
-        <v>2981</v>
+        <v>2982</v>
       </c>
       <c r="H11">
         <v>2932</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -817,14 +817,14 @@
         <v>20</v>
       </c>
       <c r="G12">
-        <v>2772</v>
+        <v>2773</v>
       </c>
       <c r="H12">
         <v>3049</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>-277</v>
+        <v>-276</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -847,14 +847,14 @@
         <v>21</v>
       </c>
       <c r="G13">
-        <v>2768</v>
+        <v>2769</v>
       </c>
       <c r="H13">
         <v>2810</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>-42</v>
+        <v>-41</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -967,14 +967,14 @@
         <v>25</v>
       </c>
       <c r="G17">
-        <v>2690</v>
+        <v>2691</v>
       </c>
       <c r="H17">
         <v>2891</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>-201</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1027,14 +1027,14 @@
         <v>27</v>
       </c>
       <c r="G19">
-        <v>2633</v>
+        <v>2635</v>
       </c>
       <c r="H19">
         <v>2835</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>-202</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,14 +1057,14 @@
         <v>28</v>
       </c>
       <c r="G20">
-        <v>2610</v>
+        <v>2612</v>
       </c>
       <c r="H20">
         <v>2855</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>-245</v>
+        <v>-243</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1086,14 +1086,14 @@
         <v>29</v>
       </c>
       <c r="G21">
-        <v>2519</v>
+        <v>2520</v>
       </c>
       <c r="H21">
         <v>2848</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>-329</v>
+        <v>-328</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,14 +1115,14 @@
         <v>30</v>
       </c>
       <c r="G22">
-        <v>2666</v>
+        <v>2668</v>
       </c>
       <c r="H22">
         <v>2835</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>-169</v>
+        <v>-167</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1130,14 +1130,14 @@
         <v>31</v>
       </c>
       <c r="G23">
-        <v>2640</v>
+        <v>2641</v>
       </c>
       <c r="H23">
         <v>2944</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>-304</v>
+        <v>-303</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1145,14 +1145,14 @@
         <v>32</v>
       </c>
       <c r="G24">
-        <v>2623</v>
+        <v>2625</v>
       </c>
       <c r="H24">
         <v>3103</v>
       </c>
       <c r="I24">
-        <f>G24-H24</f>
-        <v>-480</v>
+        <f t="shared" si="0"/>
+        <v>-478</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,14 +1160,29 @@
         <v>33</v>
       </c>
       <c r="G25">
-        <v>3172</v>
+        <v>3189</v>
       </c>
       <c r="H25">
         <v>3114</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>34</v>
+      </c>
+      <c r="G26">
+        <v>2810</v>
+      </c>
+      <c r="H26">
+        <v>3022</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>-212</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,16 +1190,16 @@
         <v>7</v>
       </c>
       <c r="G28" s="3">
-        <f>SUM(G3:G25)</f>
-        <v>73758</v>
+        <f t="shared" ref="G28:H28" si="2">SUM(G3:G26)</f>
+        <v>76599</v>
       </c>
       <c r="H28" s="3">
-        <f>SUM(H3:H25)</f>
-        <v>67960</v>
+        <f t="shared" si="2"/>
+        <v>70982</v>
       </c>
       <c r="I28" s="3">
-        <f>SUM(I3:I25)</f>
-        <v>5798</v>
+        <f>SUM(I3:I26)</f>
+        <v>5617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excess mortality analysis to week 35
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>3052</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I26" si="0">G3-H3</f>
+        <f t="shared" ref="I3:I27" si="0">G3-H3</f>
         <v>164</v>
       </c>
     </row>
@@ -612,14 +612,14 @@
         <v>12</v>
       </c>
       <c r="G4">
-        <v>3612</v>
+        <v>3613</v>
       </c>
       <c r="H4">
         <v>3093</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -687,14 +687,14 @@
         <v>15</v>
       </c>
       <c r="G7">
-        <v>4977</v>
+        <v>4978</v>
       </c>
       <c r="H7">
         <v>2908</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>2069</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -907,14 +907,14 @@
         <v>23</v>
       </c>
       <c r="G15">
-        <v>2681</v>
+        <v>2682</v>
       </c>
       <c r="H15">
         <v>2860</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>-179</v>
+        <v>-178</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1086,14 +1086,14 @@
         <v>29</v>
       </c>
       <c r="G21">
-        <v>2520</v>
+        <v>2523</v>
       </c>
       <c r="H21">
         <v>2848</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>-328</v>
+        <v>-325</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,14 +1115,14 @@
         <v>30</v>
       </c>
       <c r="G22">
-        <v>2668</v>
+        <v>2669</v>
       </c>
       <c r="H22">
         <v>2835</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>-167</v>
+        <v>-166</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1130,14 +1130,14 @@
         <v>31</v>
       </c>
       <c r="G23">
-        <v>2641</v>
+        <v>2651</v>
       </c>
       <c r="H23">
         <v>2944</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>-303</v>
+        <v>-293</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1145,14 +1145,14 @@
         <v>32</v>
       </c>
       <c r="G24">
-        <v>2625</v>
+        <v>2628</v>
       </c>
       <c r="H24">
         <v>3103</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>-478</v>
+        <v>-475</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,14 +1160,14 @@
         <v>33</v>
       </c>
       <c r="G25">
-        <v>3189</v>
+        <v>3197</v>
       </c>
       <c r="H25">
         <v>3114</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,31 +1175,46 @@
         <v>34</v>
       </c>
       <c r="G26">
-        <v>2810</v>
+        <v>2821</v>
       </c>
       <c r="H26">
         <v>3022</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>-212</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+        <v>-201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>35</v>
+      </c>
+      <c r="G27">
+        <v>2689</v>
+      </c>
+      <c r="H27">
+        <v>2822</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>-133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>7</v>
       </c>
-      <c r="G28" s="3">
-        <f t="shared" ref="G28:H28" si="2">SUM(G3:G26)</f>
-        <v>76599</v>
-      </c>
-      <c r="H28" s="3">
+      <c r="G29" s="3">
+        <f>SUM(G3:G27)</f>
+        <v>79327</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" ref="H29:I29" si="2">SUM(H3:H27)</f>
+        <v>73804</v>
+      </c>
+      <c r="I29" s="3">
         <f t="shared" si="2"/>
-        <v>70982</v>
-      </c>
-      <c r="I28" s="3">
-        <f>SUM(I3:I26)</f>
-        <v>5617</v>
+        <v>5523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excess mortality analyses
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,7 @@
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="10" max="1023" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -587,14 +587,14 @@
         <v>11</v>
       </c>
       <c r="G3">
-        <v>3216</v>
+        <v>3217</v>
       </c>
       <c r="H3">
         <v>3052</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I28" si="0">G3-H3</f>
-        <v>164</v>
+        <f t="shared" ref="I3:I29" si="0">G3-H3</f>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -612,14 +612,14 @@
         <v>12</v>
       </c>
       <c r="G4">
-        <v>3613</v>
+        <v>3615</v>
       </c>
       <c r="H4">
         <v>3093</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -637,14 +637,14 @@
         <v>13</v>
       </c>
       <c r="G5">
-        <v>4458</v>
+        <v>4459</v>
       </c>
       <c r="H5">
         <v>3114</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>1344</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -690,11 +690,11 @@
         <v>4978</v>
       </c>
       <c r="H7">
-        <v>2908</v>
+        <v>2909</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -715,11 +715,11 @@
         <v>4299</v>
       </c>
       <c r="H8">
-        <v>3009</v>
+        <v>3010</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -737,14 +737,14 @@
         <v>17</v>
       </c>
       <c r="G9">
-        <v>3905</v>
+        <v>3906</v>
       </c>
       <c r="H9">
         <v>2925</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -787,14 +787,14 @@
         <v>19</v>
       </c>
       <c r="G11">
-        <v>2982</v>
+        <v>2984</v>
       </c>
       <c r="H11">
-        <v>2932</v>
+        <v>2933</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -820,11 +820,11 @@
         <v>2773</v>
       </c>
       <c r="H12">
-        <v>3049</v>
+        <v>3050</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>-276</v>
+        <v>-277</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -847,14 +847,14 @@
         <v>21</v>
       </c>
       <c r="G13">
-        <v>2769</v>
+        <v>2770</v>
       </c>
       <c r="H13">
         <v>2810</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>-41</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -877,14 +877,14 @@
         <v>22</v>
       </c>
       <c r="G14">
-        <v>2724</v>
+        <v>2725</v>
       </c>
       <c r="H14">
         <v>2822</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>-98</v>
+        <v>-97</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -967,14 +967,14 @@
         <v>25</v>
       </c>
       <c r="G17">
-        <v>2691</v>
+        <v>2692</v>
       </c>
       <c r="H17">
         <v>2891</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>-200</v>
+        <v>-199</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1027,14 +1027,14 @@
         <v>27</v>
       </c>
       <c r="G19">
-        <v>2635</v>
+        <v>2636</v>
       </c>
       <c r="H19">
         <v>2835</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>-200</v>
+        <v>-199</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,14 +1057,14 @@
         <v>28</v>
       </c>
       <c r="G20">
-        <v>2612</v>
+        <v>2614</v>
       </c>
       <c r="H20">
-        <v>2855</v>
+        <v>2856</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>-243</v>
+        <v>-242</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1086,14 +1086,14 @@
         <v>29</v>
       </c>
       <c r="G21">
-        <v>2523</v>
+        <v>2526</v>
       </c>
       <c r="H21">
         <v>2848</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>-325</v>
+        <v>-322</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,14 +1115,14 @@
         <v>30</v>
       </c>
       <c r="G22">
-        <v>2669</v>
+        <v>2670</v>
       </c>
       <c r="H22">
         <v>2835</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>-166</v>
+        <v>-165</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1130,14 +1130,14 @@
         <v>31</v>
       </c>
       <c r="G23">
-        <v>2651</v>
+        <v>2657</v>
       </c>
       <c r="H23">
         <v>2944</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>-293</v>
+        <v>-287</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1145,14 +1145,14 @@
         <v>32</v>
       </c>
       <c r="G24">
-        <v>2628</v>
+        <v>2634</v>
       </c>
       <c r="H24">
         <v>3103</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>-475</v>
+        <v>-469</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,14 +1160,14 @@
         <v>33</v>
       </c>
       <c r="G25">
-        <v>3197</v>
+        <v>3202</v>
       </c>
       <c r="H25">
         <v>3114</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,14 +1175,14 @@
         <v>34</v>
       </c>
       <c r="G26">
-        <v>2821</v>
+        <v>2836</v>
       </c>
       <c r="H26">
         <v>3022</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>-201</v>
+        <v>-186</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1190,14 +1190,14 @@
         <v>35</v>
       </c>
       <c r="G27">
-        <v>2689</v>
+        <v>2715</v>
       </c>
       <c r="H27">
         <v>2822</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>-133</v>
+        <v>-107</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,31 +1205,46 @@
         <v>36</v>
       </c>
       <c r="G28">
-        <v>2644</v>
+        <v>2661</v>
       </c>
       <c r="H28">
         <v>2851</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>-207</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
+        <v>-190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>37</v>
+      </c>
+      <c r="G29">
+        <v>2704</v>
+      </c>
+      <c r="H29">
+        <v>2844</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G31" s="3">
         <f>SUM(G3:G28)</f>
-        <v>81971</v>
-      </c>
-      <c r="H30" s="3">
+        <v>82063</v>
+      </c>
+      <c r="H31" s="3">
         <f>SUM(H3:H28)</f>
-        <v>76655</v>
-      </c>
-      <c r="I30" s="3">
+        <v>76660</v>
+      </c>
+      <c r="I31" s="3">
         <f>SUM(I3:I28)</f>
-        <v>5316</v>
+        <v>5403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update weekly excess mortality (week 38)
Former-commit-id: 24d1c342663b2e12e2e98c69381183345b736015
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,7 @@
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="1023" width="8.7109375" customWidth="1"/>
+    <col min="10" max="1021" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -590,11 +590,11 @@
         <v>3217</v>
       </c>
       <c r="H3">
-        <v>3052</v>
+        <v>3253</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I29" si="0">G3-H3</f>
-        <v>165</v>
+        <f t="shared" ref="I3:I30" si="0">G3-H3</f>
+        <v>-36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -615,11 +615,11 @@
         <v>3615</v>
       </c>
       <c r="H4">
-        <v>3093</v>
+        <v>3174</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>522</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -640,11 +640,11 @@
         <v>4459</v>
       </c>
       <c r="H5">
-        <v>3114</v>
+        <v>3104</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>1345</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -665,11 +665,11 @@
         <v>5084</v>
       </c>
       <c r="H6">
-        <v>3114</v>
+        <v>3024</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>1970</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -687,14 +687,14 @@
         <v>15</v>
       </c>
       <c r="G7">
-        <v>4978</v>
+        <v>4979</v>
       </c>
       <c r="H7">
-        <v>2909</v>
+        <v>2957</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>2069</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -712,14 +712,14 @@
         <v>16</v>
       </c>
       <c r="G8">
-        <v>4299</v>
+        <v>4300</v>
       </c>
       <c r="H8">
-        <v>3010</v>
+        <v>2915</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>1289</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -737,14 +737,14 @@
         <v>17</v>
       </c>
       <c r="G9">
-        <v>3906</v>
+        <v>3907</v>
       </c>
       <c r="H9">
-        <v>2925</v>
+        <v>2869</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>981</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -765,11 +765,11 @@
         <v>3378</v>
       </c>
       <c r="H10">
-        <v>2978</v>
+        <v>2841</v>
       </c>
       <c r="I10">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -790,11 +790,11 @@
         <v>2984</v>
       </c>
       <c r="H11">
-        <v>2933</v>
+        <v>2821</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -820,11 +820,11 @@
         <v>2773</v>
       </c>
       <c r="H12">
-        <v>3050</v>
+        <v>2794</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>-277</v>
+        <v>-21</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -850,11 +850,11 @@
         <v>2770</v>
       </c>
       <c r="H13">
-        <v>2810</v>
+        <v>2770</v>
       </c>
       <c r="I13">
         <f t="shared" si="0"/>
-        <v>-40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -880,11 +880,11 @@
         <v>2725</v>
       </c>
       <c r="H14">
-        <v>2822</v>
+        <v>2753</v>
       </c>
       <c r="I14">
         <f t="shared" si="0"/>
-        <v>-97</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -910,11 +910,11 @@
         <v>2682</v>
       </c>
       <c r="H15">
-        <v>2860</v>
+        <v>2735</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>-178</v>
+        <v>-53</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -940,11 +940,11 @@
         <v>2691</v>
       </c>
       <c r="H16">
-        <v>2806</v>
+        <v>2737</v>
       </c>
       <c r="I16">
         <f t="shared" si="0"/>
-        <v>-115</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -970,11 +970,11 @@
         <v>2692</v>
       </c>
       <c r="H17">
-        <v>2891</v>
+        <v>2725</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>-199</v>
+        <v>-33</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1000,11 +1000,11 @@
         <v>2659</v>
       </c>
       <c r="H18">
-        <v>3063</v>
+        <v>2717</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>-404</v>
+        <v>-58</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1030,11 +1030,11 @@
         <v>2636</v>
       </c>
       <c r="H19">
-        <v>2835</v>
+        <v>2723</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>-199</v>
+        <v>-87</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,14 +1057,14 @@
         <v>28</v>
       </c>
       <c r="G20">
-        <v>2614</v>
+        <v>2616</v>
       </c>
       <c r="H20">
-        <v>2856</v>
+        <v>2719</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>-242</v>
+        <v>-103</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1089,11 +1089,11 @@
         <v>2526</v>
       </c>
       <c r="H21">
-        <v>2848</v>
+        <v>2720</v>
       </c>
       <c r="I21">
         <f t="shared" si="0"/>
-        <v>-322</v>
+        <v>-194</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1118,11 +1118,11 @@
         <v>2670</v>
       </c>
       <c r="H22">
-        <v>2835</v>
+        <v>2707</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>-165</v>
+        <v>-37</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1130,14 +1130,14 @@
         <v>31</v>
       </c>
       <c r="G23">
-        <v>2657</v>
+        <v>2658</v>
       </c>
       <c r="H23">
-        <v>2944</v>
+        <v>2687</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>-287</v>
+        <v>-29</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1148,11 +1148,11 @@
         <v>2634</v>
       </c>
       <c r="H24">
-        <v>3103</v>
+        <v>2682</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>-469</v>
+        <v>-48</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,14 +1160,14 @@
         <v>33</v>
       </c>
       <c r="G25">
-        <v>3202</v>
+        <v>3203</v>
       </c>
       <c r="H25">
-        <v>3114</v>
+        <v>2669</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>534</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1178,11 +1178,11 @@
         <v>2836</v>
       </c>
       <c r="H26">
-        <v>3022</v>
+        <v>2663</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>-186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1190,14 +1190,14 @@
         <v>35</v>
       </c>
       <c r="G27">
-        <v>2715</v>
+        <v>2720</v>
       </c>
       <c r="H27">
-        <v>2822</v>
+        <v>2667</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>-107</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,14 +1205,14 @@
         <v>36</v>
       </c>
       <c r="G28">
-        <v>2661</v>
+        <v>2668</v>
       </c>
       <c r="H28">
-        <v>2851</v>
+        <v>2676</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>-190</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1220,31 +1220,46 @@
         <v>37</v>
       </c>
       <c r="G29">
-        <v>2704</v>
+        <v>2718</v>
       </c>
       <c r="H29">
-        <v>2844</v>
+        <v>2698</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>-140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>38</v>
+      </c>
+      <c r="G30">
+        <v>2683</v>
+      </c>
+      <c r="H30">
+        <v>2729</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>-46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>7</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G32" s="3">
         <f>SUM(G3:G28)</f>
-        <v>82063</v>
-      </c>
-      <c r="H31" s="3">
+        <v>82082</v>
+      </c>
+      <c r="H32" s="3">
         <f>SUM(H3:H28)</f>
-        <v>76660</v>
-      </c>
-      <c r="I31" s="3">
+        <v>73102</v>
+      </c>
+      <c r="I32" s="3">
         <f>SUM(I3:I28)</f>
-        <v>5403</v>
+        <v>8980</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excess mortality analyses and plots
Former-commit-id: 4e82bb28e6109e2d9dbe44ee32c58ec1ad9083aa
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>3253</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I30" si="0">G3-H3</f>
+        <f t="shared" ref="I3:I32" si="0">G3-H3</f>
         <v>-36</v>
       </c>
     </row>
@@ -787,14 +787,14 @@
         <v>19</v>
       </c>
       <c r="G11">
-        <v>2984</v>
+        <v>2985</v>
       </c>
       <c r="H11">
         <v>2821</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -817,14 +817,14 @@
         <v>20</v>
       </c>
       <c r="G12">
-        <v>2773</v>
+        <v>2774</v>
       </c>
       <c r="H12">
         <v>2794</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
-        <v>-21</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -967,14 +967,14 @@
         <v>25</v>
       </c>
       <c r="G17">
-        <v>2692</v>
+        <v>2693</v>
       </c>
       <c r="H17">
         <v>2725</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>-33</v>
+        <v>-32</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,14 +1057,14 @@
         <v>28</v>
       </c>
       <c r="G20">
-        <v>2616</v>
+        <v>2617</v>
       </c>
       <c r="H20">
         <v>2719</v>
       </c>
       <c r="I20">
         <f t="shared" si="0"/>
-        <v>-103</v>
+        <v>-102</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,14 +1115,14 @@
         <v>30</v>
       </c>
       <c r="G22">
-        <v>2670</v>
+        <v>2671</v>
       </c>
       <c r="H22">
         <v>2707</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>-37</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1145,14 +1145,14 @@
         <v>32</v>
       </c>
       <c r="G24">
-        <v>2634</v>
+        <v>2635</v>
       </c>
       <c r="H24">
         <v>2682</v>
       </c>
       <c r="I24">
         <f t="shared" si="0"/>
-        <v>-48</v>
+        <v>-47</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,14 +1160,14 @@
         <v>33</v>
       </c>
       <c r="G25">
-        <v>3203</v>
+        <v>3204</v>
       </c>
       <c r="H25">
         <v>2669</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,14 +1175,14 @@
         <v>34</v>
       </c>
       <c r="G26">
-        <v>2836</v>
+        <v>2842</v>
       </c>
       <c r="H26">
         <v>2663</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1190,14 +1190,14 @@
         <v>35</v>
       </c>
       <c r="G27">
-        <v>2720</v>
+        <v>2725</v>
       </c>
       <c r="H27">
         <v>2667</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,14 +1205,14 @@
         <v>36</v>
       </c>
       <c r="G28">
-        <v>2668</v>
+        <v>2672</v>
       </c>
       <c r="H28">
         <v>2676</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1220,14 +1220,14 @@
         <v>37</v>
       </c>
       <c r="G29">
-        <v>2718</v>
+        <v>2727</v>
       </c>
       <c r="H29">
         <v>2698</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1235,31 +1235,61 @@
         <v>38</v>
       </c>
       <c r="G30">
-        <v>2683</v>
+        <v>2694</v>
       </c>
       <c r="H30">
         <v>2729</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>-46</v>
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>39</v>
+      </c>
+      <c r="G31">
+        <v>2865</v>
+      </c>
+      <c r="H31">
+        <v>2752</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F32" t="s">
+      <c r="F32">
+        <v>40</v>
+      </c>
+      <c r="G32">
+        <v>2998</v>
+      </c>
+      <c r="H32">
+        <v>2786</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="3">
+      <c r="G35" s="3">
         <f>SUM(G3:G28)</f>
-        <v>82082</v>
-      </c>
-      <c r="H32" s="3">
+        <v>82104</v>
+      </c>
+      <c r="H35" s="3">
         <f>SUM(H3:H28)</f>
         <v>73102</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I35" s="3">
         <f>SUM(I3:I28)</f>
-        <v>8980</v>
+        <v>9002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update weekly excess mortality
Former-commit-id: 9a2ba0925d39911d22ddba7a354b2ece656c1152
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>3253</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I34" si="0">G3-H3</f>
+        <f t="shared" ref="I3:I35" si="0">G3-H3</f>
         <v>-36</v>
       </c>
     </row>
@@ -712,14 +712,14 @@
         <v>16</v>
       </c>
       <c r="G8">
-        <v>4303</v>
+        <v>4304</v>
       </c>
       <c r="H8">
         <v>2915</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>1388</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,14 +1160,14 @@
         <v>33</v>
       </c>
       <c r="G25">
-        <v>3206</v>
+        <v>3207</v>
       </c>
       <c r="H25">
         <v>2669</v>
       </c>
       <c r="I25">
         <f t="shared" si="0"/>
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1175,14 +1175,14 @@
         <v>34</v>
       </c>
       <c r="G26">
-        <v>2845</v>
+        <v>2846</v>
       </c>
       <c r="H26">
         <v>2663</v>
       </c>
       <c r="I26">
         <f t="shared" si="0"/>
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,14 +1205,14 @@
         <v>36</v>
       </c>
       <c r="G28">
-        <v>2679</v>
+        <v>2682</v>
       </c>
       <c r="H28">
         <v>2676</v>
       </c>
       <c r="I28">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1220,14 +1220,14 @@
         <v>37</v>
       </c>
       <c r="G29">
-        <v>2733</v>
+        <v>2734</v>
       </c>
       <c r="H29">
         <v>2698</v>
       </c>
       <c r="I29">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1235,14 +1235,14 @@
         <v>38</v>
       </c>
       <c r="G30">
-        <v>2710</v>
+        <v>2712</v>
       </c>
       <c r="H30">
         <v>2729</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>-19</v>
+        <v>-17</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1250,14 +1250,14 @@
         <v>39</v>
       </c>
       <c r="G31">
-        <v>2881</v>
+        <v>2883</v>
       </c>
       <c r="H31">
         <v>2752</v>
       </c>
       <c r="I31">
         <f t="shared" si="0"/>
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1265,14 +1265,14 @@
         <v>40</v>
       </c>
       <c r="G32">
-        <v>2988</v>
+        <v>2993</v>
       </c>
       <c r="H32">
         <v>2786</v>
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
@@ -1280,14 +1280,14 @@
         <v>41</v>
       </c>
       <c r="G33">
-        <v>2996</v>
+        <v>3005</v>
       </c>
       <c r="H33">
         <v>2807</v>
       </c>
       <c r="I33">
         <f t="shared" si="0"/>
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
@@ -1295,14 +1295,29 @@
         <v>42</v>
       </c>
       <c r="G34">
-        <v>3224</v>
+        <v>3197</v>
       </c>
       <c r="H34">
         <v>2839</v>
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>385</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>43</v>
+      </c>
+      <c r="G35">
+        <v>3452</v>
+      </c>
+      <c r="H35">
+        <v>2862</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>590</v>
       </c>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
@@ -1311,7 +1326,7 @@
       </c>
       <c r="G37" s="3">
         <f>SUM(G3:G28)</f>
-        <v>82134</v>
+        <v>82140</v>
       </c>
       <c r="H37" s="3">
         <f>SUM(H3:H28)</f>
@@ -1319,7 +1334,7 @@
       </c>
       <c r="I37" s="3">
         <f>SUM(I3:I34)</f>
-        <v>9953</v>
+        <v>9951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excess mortality week 44
Former-commit-id: d7caa49acc414cc2c5e29ebbe1d8cb31736588a9
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -513,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>3253</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I35" si="0">G3-H3</f>
+        <f t="shared" ref="I3:I36" si="0">G3-H3</f>
         <v>-36</v>
       </c>
     </row>
@@ -1320,19 +1320,34 @@
         <v>590</v>
       </c>
     </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F37" t="s">
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>44</v>
+      </c>
+      <c r="G36">
+        <v>3617</v>
+      </c>
+      <c r="H36">
+        <v>2889</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>728</v>
+      </c>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
         <v>7</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G40" s="3">
         <f>SUM(G3:G28)</f>
         <v>82140</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H40" s="3">
         <f>SUM(H3:H28)</f>
         <v>73102</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I40" s="3">
         <f>SUM(I3:I34)</f>
         <v>9951</v>
       </c>

</xml_diff>

<commit_message>
Excess mortality analyses - Week 50
Former-commit-id: 2c2bace52e4774dabe0732a212d22027278f7989
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Gem. temperatuur</t>
   </si>
@@ -51,18 +51,6 @@
   </si>
   <si>
     <t>Som week 11 tot en met 19</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -525,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +593,7 @@
         <v>3253</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I41" si="0">G3-H3</f>
+        <f t="shared" ref="I3:I42" si="0">G3-H3</f>
         <v>-34</v>
       </c>
     </row>
@@ -1127,14 +1115,14 @@
         <v>30</v>
       </c>
       <c r="G22">
-        <v>2671</v>
+        <v>2673</v>
       </c>
       <c r="H22">
         <v>2707</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>-36</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1142,14 +1130,14 @@
         <v>31</v>
       </c>
       <c r="G23">
-        <v>2667</v>
+        <v>2668</v>
       </c>
       <c r="H23">
         <v>2687</v>
       </c>
       <c r="I23">
         <f t="shared" si="0"/>
-        <v>-20</v>
+        <v>-19</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1247,14 +1235,14 @@
         <v>38</v>
       </c>
       <c r="G30">
-        <v>2718</v>
+        <v>2719</v>
       </c>
       <c r="H30">
         <v>2729</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1277,14 +1265,14 @@
         <v>40</v>
       </c>
       <c r="G32">
-        <v>2996</v>
+        <v>2997</v>
       </c>
       <c r="H32">
         <v>2786</v>
       </c>
       <c r="I32">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
@@ -1307,14 +1295,14 @@
         <v>42</v>
       </c>
       <c r="G34">
-        <v>3212</v>
+        <v>3216</v>
       </c>
       <c r="H34">
         <v>2839</v>
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="6:9" x14ac:dyDescent="0.25">
@@ -1322,14 +1310,14 @@
         <v>43</v>
       </c>
       <c r="G35">
-        <v>3444</v>
+        <v>3445</v>
       </c>
       <c r="H35">
         <v>2862</v>
       </c>
       <c r="I35">
         <f t="shared" si="0"/>
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="36" spans="6:9" x14ac:dyDescent="0.25">
@@ -1337,14 +1325,14 @@
         <v>44</v>
       </c>
       <c r="G36">
-        <v>3674</v>
+        <v>3675</v>
       </c>
       <c r="H36">
         <v>2889</v>
       </c>
       <c r="I36">
         <f t="shared" si="0"/>
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
@@ -1367,14 +1355,14 @@
         <v>46</v>
       </c>
       <c r="G38">
-        <v>3552</v>
+        <v>3560</v>
       </c>
       <c r="H38">
         <v>2932</v>
       </c>
       <c r="I38">
         <f t="shared" si="0"/>
-        <v>620</v>
+        <v>628</v>
       </c>
     </row>
     <row r="39" spans="6:9" x14ac:dyDescent="0.25">
@@ -1382,14 +1370,14 @@
         <v>47</v>
       </c>
       <c r="G39">
-        <v>3315</v>
+        <v>3317</v>
       </c>
       <c r="H39">
         <v>2972</v>
       </c>
       <c r="I39">
         <f t="shared" si="0"/>
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="40" spans="6:9" x14ac:dyDescent="0.25">
@@ -1397,14 +1385,14 @@
         <v>48</v>
       </c>
       <c r="G40">
-        <v>3373</v>
+        <v>3388</v>
       </c>
       <c r="H40">
         <v>3012</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>361</v>
+        <v>376</v>
       </c>
     </row>
     <row r="41" spans="6:9" x14ac:dyDescent="0.25">
@@ -1412,31 +1400,56 @@
         <v>49</v>
       </c>
       <c r="G41">
-        <v>3448</v>
+        <v>3494</v>
       </c>
       <c r="H41">
         <v>3037</v>
       </c>
       <c r="I41">
         <f t="shared" si="0"/>
-        <v>411</v>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>50</v>
+      </c>
+      <c r="G42">
+        <v>3571</v>
+      </c>
+      <c r="H42">
+        <v>3100</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="0"/>
+        <v>471</v>
       </c>
     </row>
     <row r="43" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F43" t="s">
+      <c r="F43">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
         <v>7</v>
       </c>
-      <c r="G43" s="3">
+      <c r="G46" s="3">
         <f>SUM(G3:G28)</f>
-        <v>82182</v>
-      </c>
-      <c r="H43" s="3">
+        <v>82185</v>
+      </c>
+      <c r="H46" s="3">
         <f>SUM(H3:H28)</f>
         <v>73102</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I46" s="3">
         <f>SUM(I3:I34)</f>
-        <v>10043</v>
+        <v>10052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excess mortality analyses - Week 52
Former-commit-id: 5b4ccab901e9a19ef59e6f847289d2ca6ae76de3
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +593,7 @@
         <v>3253</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I43" si="0">G3-H3</f>
+        <f t="shared" ref="I3:I44" si="0">G3-H3</f>
         <v>-34</v>
       </c>
     </row>
@@ -1443,6 +1443,16 @@
     <row r="44" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F44">
         <v>52</v>
+      </c>
+      <c r="G44">
+        <v>3819</v>
+      </c>
+      <c r="H44">
+        <v>3222</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>597</v>
       </c>
     </row>
     <row r="46" spans="6:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update CBS model excess mortality table
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Gem. temperatuur</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Som week 11 tot en met 19</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Jaar</t>
   </si>
 </sst>
 </file>
@@ -513,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,15 +531,15 @@
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="1021" width="8.7109375" customWidth="1"/>
+    <col min="5" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="11" max="1022" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -543,17 +549,23 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -564,15 +576,18 @@
         <f>'[1]Grafiek 1'!E4</f>
         <v>3102</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2">
+        <v>2020</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <f>AVERAGE(C4:C11)</f>
         <v>3111.25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -584,20 +599,23 @@
         <v>3364</v>
       </c>
       <c r="F3">
+        <v>2020</v>
+      </c>
+      <c r="G3">
         <v>11</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3219</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3253</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I44" si="0">G3-H3</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J46" si="0">H3-I3</f>
         <v>-34</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -609,20 +627,23 @@
         <v>3153</v>
       </c>
       <c r="F4">
+        <v>2020</v>
+      </c>
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>3615</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>3174</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>441</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -634,20 +655,23 @@
         <v>3042</v>
       </c>
       <c r="F5">
+        <v>2020</v>
+      </c>
+      <c r="G5">
         <v>13</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4459</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>3104</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>1355</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -659,20 +683,23 @@
         <v>3160</v>
       </c>
       <c r="F6">
+        <v>2020</v>
+      </c>
+      <c r="G6">
         <v>14</v>
       </c>
-      <c r="G6">
-        <v>5084</v>
-      </c>
       <c r="H6">
+        <v>5085</v>
+      </c>
+      <c r="I6">
         <v>3024</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>2060</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>2061</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -684,20 +711,23 @@
         <v>3191</v>
       </c>
       <c r="F7">
+        <v>2020</v>
+      </c>
+      <c r="G7">
         <v>15</v>
       </c>
-      <c r="G7">
-        <v>4980</v>
-      </c>
       <c r="H7">
+        <v>4981</v>
+      </c>
+      <c r="I7">
         <v>2957</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -709,20 +739,23 @@
         <v>3197</v>
       </c>
       <c r="F8">
+        <v>2020</v>
+      </c>
+      <c r="G8">
         <v>16</v>
       </c>
-      <c r="G8">
-        <v>4306</v>
-      </c>
       <c r="H8">
+        <v>4307</v>
+      </c>
+      <c r="I8">
         <v>2915</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>1391</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -734,20 +767,23 @@
         <v>2957</v>
       </c>
       <c r="F9">
+        <v>2020</v>
+      </c>
+      <c r="G9">
         <v>17</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>3907</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>2869</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>1038</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -759,20 +795,23 @@
         <v>3092</v>
       </c>
       <c r="F10">
+        <v>2020</v>
+      </c>
+      <c r="G10">
         <v>18</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>3379</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>2841</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>538</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -784,20 +823,23 @@
         <v>3098</v>
       </c>
       <c r="F11">
+        <v>2020</v>
+      </c>
+      <c r="G11">
         <v>19</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2986</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>2821</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -814,20 +856,23 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12">
+        <v>2020</v>
+      </c>
+      <c r="G12">
         <v>20</v>
       </c>
-      <c r="G12">
-        <v>2775</v>
-      </c>
       <c r="H12">
+        <v>2777</v>
+      </c>
+      <c r="I12">
         <v>2794</v>
       </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>-19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -844,20 +889,23 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13">
+        <v>2020</v>
+      </c>
+      <c r="G13">
         <v>21</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>2771</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2770</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -874,20 +922,23 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14">
+        <v>2020</v>
+      </c>
+      <c r="G14">
         <v>22</v>
       </c>
-      <c r="G14">
-        <v>2728</v>
-      </c>
       <c r="H14">
+        <v>2729</v>
+      </c>
+      <c r="I14">
         <v>2753</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="0"/>
-        <v>-25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -904,20 +955,23 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15">
+        <v>2020</v>
+      </c>
+      <c r="G15">
         <v>23</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2682</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>2735</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>-53</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -934,20 +988,23 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16">
+        <v>2020</v>
+      </c>
+      <c r="G16">
         <v>24</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>2692</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>2737</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>-45</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -964,20 +1021,23 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17">
+        <v>2020</v>
+      </c>
+      <c r="G17">
         <v>25</v>
       </c>
-      <c r="G17">
-        <v>2694</v>
-      </c>
       <c r="H17">
+        <v>2695</v>
+      </c>
+      <c r="I17">
         <v>2725</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="0"/>
-        <v>-31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -994,20 +1054,23 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18">
+        <v>2020</v>
+      </c>
+      <c r="G18">
         <v>26</v>
       </c>
-      <c r="G18">
-        <v>2660</v>
-      </c>
       <c r="H18">
+        <v>2661</v>
+      </c>
+      <c r="I18">
         <v>2717</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>-57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>-56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1024,20 +1087,23 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19">
+        <v>2020</v>
+      </c>
+      <c r="G19">
         <v>27</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>2639</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>2723</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>-84</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1054,20 +1120,23 @@
       </c>
       <c r="E20" s="3"/>
       <c r="F20">
+        <v>2020</v>
+      </c>
+      <c r="G20">
         <v>28</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>2619</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>2719</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>-100</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1083,20 +1152,23 @@
         <v>0.97933928571428563</v>
       </c>
       <c r="F21">
+        <v>2020</v>
+      </c>
+      <c r="G21">
         <v>29</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>2528</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>2720</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>-192</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1112,364 +1184,469 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22">
+        <v>2020</v>
+      </c>
+      <c r="G22">
         <v>30</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>2673</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>2707</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <f t="shared" si="0"/>
         <v>-34</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F23">
+        <v>2020</v>
+      </c>
+      <c r="G23">
         <v>31</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>2668</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>2687</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>-19</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F24">
+        <v>2020</v>
+      </c>
+      <c r="G24">
         <v>32</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>2640</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>2682</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f t="shared" si="0"/>
         <v>-42</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F25">
+        <v>2020</v>
+      </c>
+      <c r="G25">
         <v>33</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>3209</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>2669</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>540</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F26">
+        <v>2020</v>
+      </c>
+      <c r="G26">
         <v>34</v>
       </c>
-      <c r="G26">
-        <v>2854</v>
-      </c>
       <c r="H26">
+        <v>2855</v>
+      </c>
+      <c r="I26">
         <v>2663</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="0"/>
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F27">
+        <v>2020</v>
+      </c>
+      <c r="G27">
         <v>35</v>
       </c>
-      <c r="G27">
-        <v>2732</v>
-      </c>
       <c r="H27">
+        <v>2733</v>
+      </c>
+      <c r="I27">
         <v>2667</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F28">
+        <v>2020</v>
+      </c>
+      <c r="G28">
         <v>36</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>2690</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>2676</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F29">
+        <v>2020</v>
+      </c>
+      <c r="G29">
         <v>37</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>2739</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>2698</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F30">
+        <v>2020</v>
+      </c>
+      <c r="G30">
         <v>38</v>
       </c>
-      <c r="G30">
-        <v>2719</v>
-      </c>
       <c r="H30">
+        <v>2720</v>
+      </c>
+      <c r="I30">
         <v>2729</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F31">
+        <v>2020</v>
+      </c>
+      <c r="G31">
         <v>39</v>
       </c>
-      <c r="G31">
-        <v>2891</v>
-      </c>
       <c r="H31">
+        <v>2892</v>
+      </c>
+      <c r="I31">
         <v>2752</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F32">
+        <v>2020</v>
+      </c>
+      <c r="G32">
         <v>40</v>
       </c>
-      <c r="G32">
-        <v>2997</v>
-      </c>
       <c r="H32">
+        <v>2998</v>
+      </c>
+      <c r="I32">
         <v>2786</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="0"/>
-        <v>211</v>
-      </c>
-    </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F33">
+        <v>2020</v>
+      </c>
+      <c r="G33">
         <v>41</v>
       </c>
-      <c r="G33">
-        <v>3019</v>
-      </c>
       <c r="H33">
+        <v>3020</v>
+      </c>
+      <c r="I33">
         <v>2807</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="0"/>
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F34">
+        <v>2020</v>
+      </c>
+      <c r="G34">
         <v>42</v>
       </c>
-      <c r="G34">
-        <v>3217</v>
-      </c>
       <c r="H34">
+        <v>3220</v>
+      </c>
+      <c r="I34">
         <v>2839</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="0"/>
-        <v>378</v>
-      </c>
-    </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>381</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F35">
+        <v>2020</v>
+      </c>
+      <c r="G35">
         <v>43</v>
       </c>
-      <c r="G35">
-        <v>3448</v>
-      </c>
       <c r="H35">
+        <v>3449</v>
+      </c>
+      <c r="I35">
         <v>2862</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="0"/>
-        <v>586</v>
-      </c>
-    </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>587</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F36">
+        <v>2020</v>
+      </c>
+      <c r="G36">
         <v>44</v>
       </c>
-      <c r="G36">
-        <v>3676</v>
-      </c>
       <c r="H36">
+        <v>3679</v>
+      </c>
+      <c r="I36">
         <v>2889</v>
       </c>
-      <c r="I36">
-        <f t="shared" si="0"/>
-        <v>787</v>
-      </c>
-    </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>790</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F37">
+        <v>2020</v>
+      </c>
+      <c r="G37">
         <v>45</v>
       </c>
-      <c r="G37">
-        <v>3587</v>
-      </c>
       <c r="H37">
+        <v>3589</v>
+      </c>
+      <c r="I37">
         <v>2902</v>
       </c>
-      <c r="I37">
-        <f t="shared" si="0"/>
-        <v>685</v>
-      </c>
-    </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>687</v>
+      </c>
+    </row>
+    <row r="38" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F38">
+        <v>2020</v>
+      </c>
+      <c r="G38">
         <v>46</v>
       </c>
-      <c r="G38">
-        <v>3566</v>
-      </c>
       <c r="H38">
+        <v>3575</v>
+      </c>
+      <c r="I38">
         <v>2932</v>
       </c>
-      <c r="I38">
-        <f t="shared" si="0"/>
-        <v>634</v>
-      </c>
-    </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F39">
+        <v>2020</v>
+      </c>
+      <c r="G39">
         <v>47</v>
       </c>
-      <c r="G39">
-        <v>3324</v>
-      </c>
       <c r="H39">
+        <v>3329</v>
+      </c>
+      <c r="I39">
         <v>2972</v>
       </c>
-      <c r="I39">
-        <f t="shared" si="0"/>
-        <v>352</v>
-      </c>
-    </row>
-    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="40" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F40">
+        <v>2020</v>
+      </c>
+      <c r="G40">
         <v>48</v>
       </c>
-      <c r="G40">
-        <v>3393</v>
-      </c>
       <c r="H40">
+        <v>3401</v>
+      </c>
+      <c r="I40">
         <v>3012</v>
       </c>
-      <c r="I40">
-        <f t="shared" si="0"/>
-        <v>381</v>
-      </c>
-    </row>
-    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <f t="shared" si="0"/>
+        <v>389</v>
+      </c>
+    </row>
+    <row r="41" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F41">
+        <v>2020</v>
+      </c>
+      <c r="G41">
         <v>49</v>
       </c>
-      <c r="G41">
-        <v>3512</v>
-      </c>
       <c r="H41">
+        <v>3519</v>
+      </c>
+      <c r="I41">
         <v>3037</v>
       </c>
-      <c r="I41">
-        <f t="shared" si="0"/>
-        <v>475</v>
-      </c>
-    </row>
-    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <f t="shared" si="0"/>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="42" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F42">
+        <v>2020</v>
+      </c>
+      <c r="G42">
         <v>50</v>
       </c>
-      <c r="G42">
-        <v>3580</v>
-      </c>
       <c r="H42">
+        <v>3606</v>
+      </c>
+      <c r="I42">
         <v>3100</v>
       </c>
-      <c r="I42">
-        <f t="shared" si="0"/>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <f t="shared" si="0"/>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="43" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F43">
+        <v>2020</v>
+      </c>
+      <c r="G43">
         <v>51</v>
       </c>
-      <c r="G43">
-        <v>3959</v>
-      </c>
       <c r="H43">
+        <v>3896</v>
+      </c>
+      <c r="I43">
         <v>3166</v>
       </c>
-      <c r="I43">
-        <f t="shared" si="0"/>
-        <v>793</v>
-      </c>
-    </row>
-    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <f t="shared" si="0"/>
+        <v>730</v>
+      </c>
+    </row>
+    <row r="44" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F44">
+        <v>2020</v>
+      </c>
+      <c r="G44">
         <v>52</v>
       </c>
-      <c r="G44">
-        <v>3819</v>
-      </c>
       <c r="H44">
+        <v>3849</v>
+      </c>
+      <c r="I44">
         <v>3222</v>
       </c>
-      <c r="I44">
-        <f t="shared" si="0"/>
-        <v>597</v>
-      </c>
-    </row>
-    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F46" t="s">
+      <c r="J44">
+        <f t="shared" si="0"/>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="45" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>2020</v>
+      </c>
+      <c r="G45">
+        <v>53</v>
+      </c>
+      <c r="H45">
+        <v>4058</v>
+      </c>
+      <c r="I45">
+        <v>3266</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="0"/>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="46" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>2021</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>3954</v>
+      </c>
+      <c r="I46">
+        <v>3309</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="0"/>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="3">
-        <f>SUM(G3:G28)</f>
-        <v>82189</v>
-      </c>
-      <c r="H46" s="3">
+      <c r="H50" s="3">
         <f>SUM(H3:H28)</f>
+        <v>82199</v>
+      </c>
+      <c r="I50" s="3">
+        <f>SUM(I3:I28)</f>
         <v>73102</v>
       </c>
-      <c r="I46" s="3">
-        <f>SUM(I3:I34)</f>
-        <v>10058</v>
+      <c r="J50" s="3">
+        <f>SUM(J3:J34)</f>
+        <v>10075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update excess mortality CBS model
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Gem. temperatuur</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>3-10</t>
-  </si>
-  <si>
-    <t>Som week 11 tot en met 19</t>
   </si>
   <si>
     <t>Week</t>
@@ -519,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,10 +547,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -611,7 +608,7 @@
         <v>3253</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J46" si="0">H3-I3</f>
+        <f t="shared" ref="J3:J49" si="0">H3-I3</f>
         <v>-34</v>
       </c>
     </row>
@@ -1604,14 +1601,14 @@
         <v>53</v>
       </c>
       <c r="H45">
-        <v>4058</v>
+        <v>4077</v>
       </c>
       <c r="I45">
         <v>3266</v>
       </c>
       <c r="J45">
         <f t="shared" si="0"/>
-        <v>792</v>
+        <v>811</v>
       </c>
     </row>
     <row r="46" spans="6:10" x14ac:dyDescent="0.25">
@@ -1622,32 +1619,74 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>3954</v>
+        <v>4118</v>
       </c>
       <c r="I46">
         <v>3309</v>
       </c>
       <c r="J46">
         <f t="shared" si="0"/>
-        <v>645</v>
-      </c>
-    </row>
-    <row r="50" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G50" t="s">
-        <v>7</v>
-      </c>
-      <c r="H50" s="3">
-        <f>SUM(H3:H28)</f>
-        <v>82199</v>
-      </c>
-      <c r="I50" s="3">
-        <f>SUM(I3:I28)</f>
-        <v>73102</v>
-      </c>
-      <c r="J50" s="3">
-        <f>SUM(J3:J34)</f>
-        <v>10075</v>
-      </c>
+        <v>809</v>
+      </c>
+    </row>
+    <row r="47" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>2021</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>3825</v>
+      </c>
+      <c r="I47">
+        <v>3343</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="0"/>
+        <v>482</v>
+      </c>
+    </row>
+    <row r="48" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>2021</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>3823</v>
+      </c>
+      <c r="I48">
+        <v>3376</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="0"/>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>2021</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
+      <c r="H49">
+        <v>3758</v>
+      </c>
+      <c r="I49">
+        <v>3425</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="0"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Update CBS Oversterfte data
</commit_message>
<xml_diff>
--- a/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
+++ b/workflow/excess_mortality/data/Berekening oversterfte CBS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s379011\surfdrive\projects\2020covid-19\covid-19\workflow\excess_mortality\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD9CCC5-DDE3-45B0-A2ED-DE58FA921515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Berekening oversterfte" sheetId="1" r:id="rId1"/>
@@ -17,8 +18,16 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -59,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -515,11 +524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,10 +1692,185 @@
         <v>333</v>
       </c>
     </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>2021</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>3758</v>
+      </c>
+      <c r="I50">
+        <v>3425</v>
+      </c>
+      <c r="J50">
+        <f t="shared" ref="J50:J59" si="2">H50-I50</f>
+        <v>333</v>
+      </c>
+    </row>
     <row r="51" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="F51">
+        <v>2021</v>
+      </c>
+      <c r="G51">
+        <v>6</v>
+      </c>
+      <c r="H51">
+        <v>3758</v>
+      </c>
+      <c r="I51">
+        <v>3425</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>2021</v>
+      </c>
+      <c r="G52">
+        <v>7</v>
+      </c>
+      <c r="H52">
+        <v>3758</v>
+      </c>
+      <c r="I52">
+        <v>3425</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="53" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>2021</v>
+      </c>
+      <c r="G53">
+        <v>8</v>
+      </c>
+      <c r="H53">
+        <v>3758</v>
+      </c>
+      <c r="I53">
+        <v>3425</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>2021</v>
+      </c>
+      <c r="G54">
+        <v>9</v>
+      </c>
+      <c r="H54">
+        <v>3758</v>
+      </c>
+      <c r="I54">
+        <v>3425</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>2021</v>
+      </c>
+      <c r="G55">
+        <v>10</v>
+      </c>
+      <c r="H55">
+        <v>3758</v>
+      </c>
+      <c r="I55">
+        <v>3425</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="56" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>2021</v>
+      </c>
+      <c r="G56">
+        <v>11</v>
+      </c>
+      <c r="H56">
+        <v>3758</v>
+      </c>
+      <c r="I56">
+        <v>3425</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>2021</v>
+      </c>
+      <c r="G57">
+        <v>12</v>
+      </c>
+      <c r="H57">
+        <v>3758</v>
+      </c>
+      <c r="I57">
+        <v>3425</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="58" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>2021</v>
+      </c>
+      <c r="G58">
+        <v>13</v>
+      </c>
+      <c r="H58">
+        <v>3758</v>
+      </c>
+      <c r="I58">
+        <v>3425</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="59" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>2021</v>
+      </c>
+      <c r="G59">
+        <v>14</v>
+      </c>
+      <c r="H59">
+        <v>3758</v>
+      </c>
+      <c r="I59">
+        <v>3425</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>